<commit_message>
Commit after add explicit wait
</commit_message>
<xml_diff>
--- a/QALegend/src/test/resources/TestData/TeamMembers.xlsx
+++ b/QALegend/src/test/resources/TestData/TeamMembers.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\git\SeliniumProject\QALegend\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A564570-03FD-40F7-8342-B39479F1439E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FEB49EB-E660-47A0-A7FC-757272298B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8206574A-2D83-463E-9C03-773DEEA7E34F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TeamMembers" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>

</xml_diff>